<commit_message>
Shopping Page test setup and a couple test cases.
</commit_message>
<xml_diff>
--- a/TestPlan.xlsx
+++ b/TestPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git_Workspaces\TestingPorfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5C0013-9B6A-43A6-85B8-CADE08EE5529}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BC7A94-DD8B-47E8-8818-52EE45E9EF0D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{65474D15-23E0-4CE5-B127-F44BC850C39A}"/>
+    <workbookView xWindow="38280" yWindow="5265" windowWidth="29040" windowHeight="15840" xr2:uid="{65474D15-23E0-4CE5-B127-F44BC850C39A}"/>
   </bookViews>
   <sheets>
     <sheet name="Selenium" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="137">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -494,6 +494,9 @@
   </si>
   <si>
     <t>Green Kart - Offers Page</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -859,802 +862,808 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01736B7F-A2A0-4AAD-A91F-D8A3A1F0F951}">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A40" sqref="A40"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="91.5703125" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" customWidth="1"/>
-    <col min="5" max="5" width="32.28515625" customWidth="1"/>
-    <col min="6" max="6" width="57.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="52.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="91.5703125" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" customWidth="1"/>
+    <col min="6" max="6" width="32.28515625" customWidth="1"/>
+    <col min="7" max="7" width="57.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="52.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3">
+        <v>136</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
+        <v>136</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5">
+    <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6">
+    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>21</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7">
+    <row r="7" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>16</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>17</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>110</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
+    <row r="8" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>18</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9">
+    <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>33</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10">
+    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
         <v>8</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
+    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11">
         <v>9</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12">
+    <row r="12" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12">
         <v>10</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s">
+    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14">
+    <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14">
         <v>12</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15">
+    <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15">
         <v>13</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16">
+    <row r="16" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16">
         <v>14</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>51</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17">
+    <row r="17" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17">
         <v>15</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>100</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18">
+    <row r="18" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18">
         <v>16</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19">
+    <row r="19" spans="2:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19">
         <v>17</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>31</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20">
+    <row r="20" spans="2:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20">
         <v>18</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>32</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21">
+    <row r="21" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21">
         <v>19</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>38</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="H21" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22">
+    <row r="22" spans="2:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22">
         <v>20</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="H22" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23">
+    <row r="23" spans="2:8" ht="150" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23">
         <v>21</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>35</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>36</v>
       </c>
-      <c r="B24">
+      <c r="C24">
         <v>22</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>37</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>36</v>
       </c>
-      <c r="B25">
+      <c r="C25">
         <v>23</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="H25" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>36</v>
       </c>
-      <c r="B26">
+      <c r="C26">
         <v>24</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>39</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="H26" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>36</v>
       </c>
-      <c r="B27">
+      <c r="C27">
         <v>25</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>53</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="H27" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>36</v>
       </c>
-      <c r="B28">
+      <c r="C28">
         <v>26</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>41</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="H28" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="29" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>36</v>
       </c>
-      <c r="B29">
+      <c r="C29">
         <v>27</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>42</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="H29" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="30" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>36</v>
       </c>
-      <c r="B30">
+      <c r="C30">
         <v>28</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>43</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>54</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="G30" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="H30" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="31" spans="2:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>36</v>
       </c>
-      <c r="B31">
+      <c r="C31">
         <v>29</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>44</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="H31" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="32" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>36</v>
       </c>
-      <c r="B32">
+      <c r="C32">
         <v>30</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>45</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="G32" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="H32" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="33" spans="2:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>46</v>
       </c>
-      <c r="B33">
+      <c r="C33">
         <v>31</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>47</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="G33" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="H33" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="34" spans="2:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
         <v>46</v>
       </c>
-      <c r="B34">
+      <c r="C34">
         <v>32</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>48</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="H34" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="35" spans="2:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>46</v>
       </c>
-      <c r="B35">
+      <c r="C35">
         <v>33</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>126</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="H35" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="36" spans="2:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>46</v>
       </c>
-      <c r="B36">
+      <c r="C36">
         <v>34</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>49</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="H36" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="37" spans="2:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
         <v>46</v>
       </c>
-      <c r="B37">
+      <c r="C37">
         <v>35</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>50</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="F37" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="G37" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="H37" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="38" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>129</v>
       </c>
-      <c r="B38">
+      <c r="C38">
         <v>36</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>130</v>
       </c>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1" t="s">
+      <c r="F38" s="1"/>
+      <c r="G38" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="H38" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="39" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>129</v>
       </c>
-      <c r="B39">
+      <c r="C39">
         <v>37</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>132</v>
       </c>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1" t="s">
+      <c r="F39" s="1"/>
+      <c r="G39" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="H39" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
         <v>135</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J3" r:id="rId1" location="/" xr:uid="{AAB5D607-33E5-4411-A2DE-CF59E7690327}"/>
+    <hyperlink ref="K3" r:id="rId1" location="/" xr:uid="{AAB5D607-33E5-4411-A2DE-CF59E7690327}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added additional tests to shopping page for Selenium.
</commit_message>
<xml_diff>
--- a/TestPlan.xlsx
+++ b/TestPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git_Workspaces\TestingPorfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BC7A94-DD8B-47E8-8818-52EE45E9EF0D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B329B40-2880-4589-98F7-2BA420E1B54A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5265" windowWidth="29040" windowHeight="15840" xr2:uid="{65474D15-23E0-4CE5-B127-F44BC850C39A}"/>
+    <workbookView xWindow="38280" yWindow="7185" windowWidth="29040" windowHeight="15720" xr2:uid="{65474D15-23E0-4CE5-B127-F44BC850C39A}"/>
   </bookViews>
   <sheets>
     <sheet name="Selenium" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="137">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -866,7 +866,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,6 +956,9 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>136</v>
+      </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
@@ -979,6 +982,9 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>136</v>
+      </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -1002,6 +1008,9 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>136</v>
+      </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>

</xml_diff>